<commit_message>
Safer logging to avoid leaking API keys
</commit_message>
<xml_diff>
--- a/plan_prompt_engineering_process.xlsx
+++ b/plan_prompt_engineering_process.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ct-rate-labeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31523557-E4DE-46E3-89B7-F8CD034B8A2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E57ECCE-E118-4B89-95B6-25A4A5AD4A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2EAB8343-9A0C-4BAE-B37B-149FC1EF4E54}"/>
+    <workbookView xWindow="-915" yWindow="3480" windowWidth="21600" windowHeight="11295" xr2:uid="{2EAB8343-9A0C-4BAE-B37B-149FC1EF4E54}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -132,21 +132,6 @@
   </si>
   <si>
     <r>
-      <t>Proof of Concept:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> F1 &gt; Baseline. (Proves examples help).</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>Error Fix:</t>
     </r>
     <r>
@@ -173,21 +158,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>Intelligence Check. Does the smarter model solve specific errors (e.g., negation) that the baseline failed? (Secondary: ROI).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">ROI (=ΔPerformance​/Δcost): </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Efficiency Check. Does the same model perform better when focused? Threshold: ΔF1&gt;0.01 for 5x the cost (since 5 labels are used).</t>
     </r>
   </si>
   <si>
@@ -224,6 +194,36 @@
   </si>
   <si>
     <t>Additional note: All tests are run 3 times. Average and std are calculated for cost, macro f1, recall and precision.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ROI (=ΔPerformance​/Δcost): </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Efficiency Check. Does the same model perform better when focused? Threshold: ΔF1&gt;0.05 for 5x the cost (since 5 labels are used).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Proof of Concept:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> F1, Recall &gt; Baseline. (Proves examples help).</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -651,7 +651,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="53.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -703,7 +703,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>9</v>
@@ -726,13 +726,13 @@
         <v>8</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -749,13 +749,13 @@
         <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -772,13 +772,13 @@
         <v>8</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -795,13 +795,13 @@
         <v>23</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -818,18 +818,18 @@
         <v>20</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>

</xml_diff>

<commit_message>
New experiment log. small change to xlsx plan dataset size.
</commit_message>
<xml_diff>
--- a/plan_prompt_engineering_process.xlsx
+++ b/plan_prompt_engineering_process.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ct-rate-labeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E57ECCE-E118-4B89-95B6-25A4A5AD4A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B002C4-805C-43E0-90A1-01AA2B15EE97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-915" yWindow="3480" windowWidth="21600" windowHeight="11295" xr2:uid="{2EAB8343-9A0C-4BAE-B37B-149FC1EF4E54}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2EAB8343-9A0C-4BAE-B37B-149FC1EF4E54}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -187,12 +187,6 @@
     <t>smallest</t>
   </si>
   <si>
-    <t>smallest (N=50)</t>
-  </si>
-  <si>
-    <t>small (N=600)</t>
-  </si>
-  <si>
     <t>Additional note: All tests are run 3 times. Average and std are calculated for cost, macro f1, recall and precision.</t>
   </si>
   <si>
@@ -224,6 +218,12 @@
       </rPr>
       <t xml:space="preserve"> F1, Recall &gt; Baseline. (Proves examples help).</t>
     </r>
+  </si>
+  <si>
+    <t>smallest (N=28)</t>
+  </si>
+  <si>
+    <t>small (N=615)</t>
   </si>
 </sst>
 </file>
@@ -651,7 +651,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="53.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -703,7 +703,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>9</v>
@@ -732,7 +732,7 @@
         <v>12</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -778,7 +778,7 @@
         <v>16</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -818,7 +818,7 @@
         <v>20</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>21</v>
@@ -829,7 +829,7 @@
     </row>
     <row r="8" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>

</xml_diff>

<commit_message>
Fixed the column VolumeName. Updated readme. fixed test fails for llm_client.py . Added script to make tiny tuning set.
</commit_message>
<xml_diff>
--- a/plan_prompt_engineering_process.xlsx
+++ b/plan_prompt_engineering_process.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ct-rate-labeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B002C4-805C-43E0-90A1-01AA2B15EE97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B6AA33-A26E-4541-ABF3-DEF429511D9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2EAB8343-9A0C-4BAE-B37B-149FC1EF4E54}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2EAB8343-9A0C-4BAE-B37B-149FC1EF4E54}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="version_1" sheetId="1" r:id="rId1"/>
+    <sheet name="version_2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="37">
   <si>
     <t>Order</t>
   </si>
@@ -224,6 +225,9 @@
   </si>
   <si>
     <t>small (N=615)</t>
+  </si>
+  <si>
+    <t>smallest (N=100)</t>
   </si>
 </sst>
 </file>
@@ -650,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05D05C95-41C7-4A59-B004-8EE8209946B0}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="53.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -842,4 +846,202 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39257FB1-A1C6-4154-86CA-31D9357094A5}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="32" customWidth="1"/>
+    <col min="7" max="7" width="54.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C8:F8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Small script for aggregating metrics in the prompt engineering process. Moved experiment logs and added one more prompt version. Minor adjustments to llm_client and evaluate_prompt to fix certain issues in the prompt engineering process.
</commit_message>
<xml_diff>
--- a/plan_prompt_engineering_process.xlsx
+++ b/plan_prompt_engineering_process.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ct-rate-labeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B6AA33-A26E-4541-ABF3-DEF429511D9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B5524A-9B4F-45B9-8D3A-814250A2A045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2EAB8343-9A0C-4BAE-B37B-149FC1EF4E54}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="39">
   <si>
     <t>Order</t>
   </si>
@@ -192,7 +192,60 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">ROI (=ΔPerformance​/Δcost): </t>
+      <t>Proof of Concept:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> F1, Recall &gt; Baseline. (Proves examples help).</t>
+    </r>
+  </si>
+  <si>
+    <t>smallest (N=28)</t>
+  </si>
+  <si>
+    <t>small (N=615)</t>
+  </si>
+  <si>
+    <t>smallest (N=100)</t>
+  </si>
+  <si>
+    <r>
+      <t>Stability:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Std Dev &lt; 0.02. (Proves valid measurement).</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Additional note: All tests are run 3 times. Average and std are calculated for cost, macro f1, recall and precision. Coverage should be ≥ 95–98%</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ΔPerformance​/Δcost: </t>
     </r>
     <r>
       <rPr>
@@ -204,30 +257,6 @@
       </rPr>
       <t>Efficiency Check. Does the same model perform better when focused? Threshold: ΔF1&gt;0.05 for 5x the cost (since 5 labels are used).</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t>Proof of Concept:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> F1, Recall &gt; Baseline. (Proves examples help).</t>
-    </r>
-  </si>
-  <si>
-    <t>smallest (N=28)</t>
-  </si>
-  <si>
-    <t>small (N=615)</t>
-  </si>
-  <si>
-    <t>smallest (N=100)</t>
   </si>
 </sst>
 </file>
@@ -655,7 +684,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="53.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -707,7 +736,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>9</v>
@@ -736,7 +765,7 @@
         <v>12</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -782,7 +811,7 @@
         <v>16</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -822,7 +851,7 @@
         <v>20</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>21</v>
@@ -853,7 +882,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,13 +932,13 @@
         <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -932,7 +961,7 @@
         <v>12</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -978,7 +1007,7 @@
         <v>16</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1018,7 +1047,7 @@
         <v>20</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>21</v>
@@ -1031,7 +1060,7 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="5" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>

</xml_diff>